<commit_message>
Implementing DDT on tests
</commit_message>
<xml_diff>
--- a/testData/TestData.xlsx
+++ b/testData/TestData.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\AutomationPythonProj\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5925"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -42,8 +42,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -71,8 +79,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,11 +382,12 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding marks of execution
</commit_message>
<xml_diff>
--- a/testData/TestData.xlsx
+++ b/testData/TestData.xlsx
@@ -24,34 +24,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Word</t>
   </si>
   <si>
     <t>ChromeDriver</t>
   </si>
-  <si>
-    <t>Expected</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -79,9 +65,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,28 +347,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>